<commit_message>
Added mapDiv variables to UnifiedLawIterations
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim_Draft_1/Code_of_Laws/UnifiedLawIteration_1.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim_Draft_1/Code_of_Laws/UnifiedLawIteration_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlg\Dropbox (ASU)\PC\Documents\GitHub\REU_MatlabSim\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim_Draft_1\Code_of_Laws\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hombo\Documents\Github Repositories\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim_Draft_1\Code_of_Laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFBA25D-3956-4973-B4B8-FF6F15BCAE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC146A64-AD15-448F-A7CE-569531D77A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="348" yWindow="300" windowWidth="14292" windowHeight="11940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Iteration" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="139">
   <si>
     <t>dt</t>
   </si>
@@ -438,6 +438,21 @@
   </si>
   <si>
     <t>verboseOutput</t>
+  </si>
+  <si>
+    <t>mapDivResolution</t>
+  </si>
+  <si>
+    <t>mapDivFrameSkip</t>
+  </si>
+  <si>
+    <t>Scores</t>
+  </si>
+  <si>
+    <t>How many boxes the map should be divided into</t>
+  </si>
+  <si>
+    <t>How often to check which divisions have been explored</t>
   </si>
 </sst>
 </file>
@@ -768,24 +783,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K96"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+      <selection activeCell="C100" sqref="A97:C100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="38.21875" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="1" max="1" width="38.19921875" customWidth="1"/>
+    <col min="2" max="2" width="23.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -796,7 +811,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -807,7 +822,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -818,7 +833,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -829,7 +844,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -840,7 +855,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -851,7 +866,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>133</v>
       </c>
@@ -859,7 +874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>95</v>
       </c>
@@ -867,7 +882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>96</v>
       </c>
@@ -875,7 +890,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>101</v>
       </c>
@@ -883,7 +898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>102</v>
       </c>
@@ -903,12 +918,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -919,7 +934,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -930,7 +945,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -941,12 +956,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -957,7 +972,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -968,7 +983,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -979,7 +994,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -990,17 +1005,17 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
         <v>34</v>
       </c>
@@ -1028,7 +1043,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>105</v>
       </c>
@@ -1036,7 +1051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -1050,7 +1065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>110</v>
       </c>
@@ -1061,7 +1076,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>112</v>
       </c>
@@ -1069,7 +1084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
         <v>113</v>
       </c>
@@ -1077,12 +1092,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
         <v>30</v>
       </c>
@@ -1099,7 +1114,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>114</v>
       </c>
@@ -1113,7 +1128,7 @@
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>115</v>
       </c>
@@ -1126,12 +1141,12 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B38" t="s">
         <v>32</v>
       </c>
@@ -1154,7 +1169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>117</v>
       </c>
@@ -1165,7 +1180,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>119</v>
       </c>
@@ -1178,7 +1193,7 @@
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>35</v>
       </c>
@@ -1186,7 +1201,7 @@
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" s="1"/>
       <c r="B42" t="s">
         <v>36</v>
@@ -1195,7 +1210,7 @@
         <v>9.9999999999999991E-22</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" s="1"/>
       <c r="B43" t="s">
         <v>121</v>
@@ -1204,12 +1219,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B45" t="s">
         <v>38</v>
       </c>
@@ -1217,7 +1232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" s="3" t="s">
         <v>41</v>
       </c>
@@ -1228,15 +1243,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" s="3"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" s="3" t="s">
         <v>99</v>
       </c>
@@ -1247,12 +1262,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>14</v>
       </c>
@@ -1263,7 +1278,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>45</v>
       </c>
@@ -1274,7 +1289,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>20</v>
       </c>
@@ -1285,7 +1300,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -1296,7 +1311,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>49</v>
       </c>
@@ -1307,7 +1322,7 @@
         <v>-0.26179938779914941</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>49</v>
       </c>
@@ -1318,7 +1333,7 @@
         <v>0.26179938779914941</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>52</v>
       </c>
@@ -1329,7 +1344,7 @@
         <v>5.7595865315812871</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B59" t="s">
         <v>53</v>
       </c>
@@ -1337,7 +1352,7 @@
         <v>-1.8429999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B60" t="s">
         <v>54</v>
       </c>
@@ -1345,7 +1360,7 @@
         <v>0.37819999999999998</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B61" t="s">
         <v>55</v>
       </c>
@@ -1353,7 +1368,7 @@
         <v>-2.3782000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -1364,12 +1379,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B65" t="s">
         <v>57</v>
       </c>
@@ -1377,7 +1392,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B66" t="s">
         <v>59</v>
       </c>
@@ -1385,7 +1400,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B67" t="s">
         <v>61</v>
       </c>
@@ -1393,7 +1408,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>65</v>
       </c>
@@ -1404,7 +1419,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B69" t="s">
         <v>66</v>
       </c>
@@ -1415,7 +1430,7 @@
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B70" t="s">
         <v>67</v>
       </c>
@@ -1423,7 +1438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B71" t="s">
         <v>68</v>
       </c>
@@ -1431,7 +1446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B72" t="s">
         <v>69</v>
       </c>
@@ -1439,7 +1454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B73" t="s">
         <v>70</v>
       </c>
@@ -1447,7 +1462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B74" t="s">
         <v>71</v>
       </c>
@@ -1455,7 +1470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>122</v>
       </c>
@@ -1466,7 +1481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B76" t="s">
         <v>123</v>
       </c>
@@ -1474,7 +1489,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B77" t="s">
         <v>104</v>
       </c>
@@ -1482,12 +1497,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A80" s="1"/>
       <c r="B80" t="s">
         <v>131</v>
@@ -1496,7 +1511,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B81" t="s">
         <v>73</v>
       </c>
@@ -1504,7 +1519,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B82" t="s">
         <v>75</v>
       </c>
@@ -1512,7 +1527,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>86</v>
       </c>
@@ -1523,7 +1538,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>20</v>
       </c>
@@ -1534,7 +1549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>20</v>
       </c>
@@ -1545,7 +1560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>14</v>
       </c>
@@ -1556,7 +1571,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>14</v>
       </c>
@@ -1567,7 +1582,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>90</v>
       </c>
@@ -1578,7 +1593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>90</v>
       </c>
@@ -1589,7 +1604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -1600,7 +1615,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>87</v>
       </c>
@@ -1611,7 +1626,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>88</v>
       </c>
@@ -1622,12 +1637,12 @@
         <v>600</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A94" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B95" t="s">
         <v>92</v>
       </c>
@@ -1635,12 +1650,39 @@
         <v>124</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B96" t="s">
         <v>93</v>
       </c>
       <c r="C96" t="s">
         <v>125</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A98" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A99" t="s">
+        <v>137</v>
+      </c>
+      <c r="B99" t="s">
+        <v>134</v>
+      </c>
+      <c r="C99">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A100" t="s">
+        <v>138</v>
+      </c>
+      <c r="B100" t="s">
+        <v>135</v>
+      </c>
+      <c r="C100">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1657,18 +1699,18 @@
       <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="38.21875" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="1" max="1" width="38.19921875" customWidth="1"/>
+    <col min="2" max="2" width="23.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1679,7 +1721,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1690,7 +1732,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1701,7 +1743,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1712,7 +1754,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1723,7 +1765,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1734,7 +1776,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>133</v>
       </c>
@@ -1742,7 +1784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>95</v>
       </c>
@@ -1750,7 +1792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>96</v>
       </c>
@@ -1758,7 +1800,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>101</v>
       </c>
@@ -1766,17 +1808,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1787,7 +1829,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1798,7 +1840,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1809,12 +1851,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1825,7 +1867,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1836,7 +1878,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1847,7 +1889,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1858,17 +1900,17 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
         <v>34</v>
       </c>
@@ -1879,7 +1921,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>105</v>
       </c>
@@ -1887,7 +1929,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -1898,7 +1940,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>110</v>
       </c>
@@ -1909,7 +1951,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>112</v>
       </c>
@@ -1917,7 +1959,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
         <v>113</v>
       </c>
@@ -1925,12 +1967,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
         <v>30</v>
       </c>
@@ -1939,7 +1981,7 @@
       </c>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>114</v>
       </c>
@@ -1953,7 +1995,7 @@
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>115</v>
       </c>
@@ -1966,12 +2008,12 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B38" t="s">
         <v>32</v>
       </c>
@@ -1979,7 +2021,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>117</v>
       </c>
@@ -1990,7 +2032,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>119</v>
       </c>
@@ -2003,7 +2045,7 @@
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>35</v>
       </c>
@@ -2011,7 +2053,7 @@
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" s="1"/>
       <c r="B42" t="s">
         <v>36</v>
@@ -2020,7 +2062,7 @@
         <v>9.9999999999999991E-22</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" s="1"/>
       <c r="B43" t="s">
         <v>121</v>
@@ -2029,12 +2071,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B45" t="s">
         <v>38</v>
       </c>
@@ -2042,7 +2084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" s="3" t="s">
         <v>41</v>
       </c>
@@ -2053,15 +2095,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" s="3"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" s="3" t="s">
         <v>99</v>
       </c>
@@ -2072,12 +2114,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>14</v>
       </c>
@@ -2088,7 +2130,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>45</v>
       </c>
@@ -2099,7 +2141,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>20</v>
       </c>
@@ -2110,7 +2152,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -2121,7 +2163,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>49</v>
       </c>
@@ -2132,7 +2174,7 @@
         <v>-0.26179938779914941</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>49</v>
       </c>
@@ -2143,7 +2185,7 @@
         <v>0.26179938779914941</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>52</v>
       </c>
@@ -2154,7 +2196,7 @@
         <v>5.7595865315812871</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B59" t="s">
         <v>53</v>
       </c>
@@ -2162,7 +2204,7 @@
         <v>-1.8429999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B60" t="s">
         <v>54</v>
       </c>
@@ -2170,7 +2212,7 @@
         <v>0.37819999999999998</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B61" t="s">
         <v>55</v>
       </c>
@@ -2178,7 +2220,7 @@
         <v>-2.3782000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -2189,12 +2231,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B65" t="s">
         <v>57</v>
       </c>
@@ -2202,7 +2244,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B66" t="s">
         <v>59</v>
       </c>
@@ -2210,7 +2252,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B67" t="s">
         <v>61</v>
       </c>
@@ -2218,7 +2260,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>65</v>
       </c>
@@ -2229,7 +2271,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B69" t="s">
         <v>66</v>
       </c>
@@ -2240,7 +2282,7 @@
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B70" t="s">
         <v>67</v>
       </c>
@@ -2248,7 +2290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B71" t="s">
         <v>68</v>
       </c>
@@ -2256,7 +2298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B72" t="s">
         <v>69</v>
       </c>
@@ -2264,7 +2306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B73" t="s">
         <v>70</v>
       </c>
@@ -2272,7 +2314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B74" t="s">
         <v>71</v>
       </c>
@@ -2280,7 +2322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>122</v>
       </c>
@@ -2291,7 +2333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B76" t="s">
         <v>123</v>
       </c>
@@ -2299,7 +2341,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B77" t="s">
         <v>104</v>
       </c>
@@ -2307,12 +2349,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A80" s="1"/>
       <c r="B80" t="s">
         <v>131</v>
@@ -2321,7 +2363,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B81" t="s">
         <v>73</v>
       </c>
@@ -2329,7 +2371,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B82" t="s">
         <v>75</v>
       </c>
@@ -2337,7 +2379,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>86</v>
       </c>
@@ -2348,7 +2390,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>20</v>
       </c>
@@ -2359,7 +2401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>20</v>
       </c>
@@ -2370,7 +2412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>14</v>
       </c>
@@ -2381,7 +2423,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>14</v>
       </c>
@@ -2392,7 +2434,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>90</v>
       </c>
@@ -2403,7 +2445,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>90</v>
       </c>
@@ -2414,7 +2456,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -2425,7 +2467,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>87</v>
       </c>
@@ -2436,7 +2478,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>88</v>
       </c>
@@ -2447,12 +2489,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A94" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B95" t="s">
         <v>92</v>
       </c>
@@ -2460,7 +2502,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B96" t="s">
         <v>93</v>
       </c>
@@ -2482,18 +2524,18 @@
       <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="38.21875" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="1" max="1" width="38.19921875" customWidth="1"/>
+    <col min="2" max="2" width="23.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -2510,7 +2552,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -2521,7 +2563,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2532,7 +2574,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2543,7 +2585,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2560,7 +2602,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2571,7 +2613,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>95</v>
       </c>
@@ -2579,7 +2621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>96</v>
       </c>
@@ -2593,7 +2635,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>101</v>
       </c>
@@ -2601,7 +2643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>102</v>
       </c>
@@ -2609,12 +2651,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -2628,7 +2670,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2639,7 +2681,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2650,12 +2692,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -2669,7 +2711,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -2683,7 +2725,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -2694,7 +2736,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -2705,17 +2747,17 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>34</v>
       </c>
@@ -2747,7 +2789,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
         <v>105</v>
       </c>
@@ -2770,7 +2812,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>108</v>
       </c>
@@ -2802,7 +2844,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>110</v>
       </c>
@@ -2834,7 +2876,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
         <v>112</v>
       </c>
@@ -2857,7 +2899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>113</v>
       </c>
@@ -2874,12 +2916,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B33" t="s">
         <v>30</v>
       </c>
@@ -2899,7 +2941,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>114</v>
       </c>
@@ -2924,7 +2966,7 @@
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>115</v>
       </c>
@@ -2956,12 +2998,12 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B37" t="s">
         <v>32</v>
       </c>
@@ -2984,7 +3026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>117</v>
       </c>
@@ -3004,7 +3046,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>119</v>
       </c>
@@ -3036,7 +3078,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>35</v>
       </c>
@@ -3049,7 +3091,7 @@
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="1"/>
       <c r="B41" t="s">
         <v>36</v>
@@ -3058,7 +3100,7 @@
         <v>9.9999999999999992E-25</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" s="1"/>
       <c r="B42" t="s">
         <v>121</v>
@@ -3070,12 +3112,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B44" t="s">
         <v>38</v>
       </c>
@@ -3083,7 +3125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" s="3" t="s">
         <v>41</v>
       </c>
@@ -3094,15 +3136,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" s="3"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" s="3" t="s">
         <v>99</v>
       </c>
@@ -3113,12 +3155,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>14</v>
       </c>
@@ -3135,7 +3177,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>45</v>
       </c>
@@ -3155,7 +3197,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>20</v>
       </c>
@@ -3166,7 +3208,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>20</v>
       </c>
@@ -3177,7 +3219,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>49</v>
       </c>
@@ -3193,7 +3235,7 @@
         <v>-0.26179938779914941</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>49</v>
       </c>
@@ -3209,7 +3251,7 @@
         <v>0.26179938779914941</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>52</v>
       </c>
@@ -3229,7 +3271,7 @@
         <v>3.1415926535897931</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B58" t="s">
         <v>53</v>
       </c>
@@ -3237,7 +3279,7 @@
         <v>-1.8429999999999998E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B59" t="s">
         <v>54</v>
       </c>
@@ -3245,7 +3287,7 @@
         <v>0.37819999999999998</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B60" t="s">
         <v>55</v>
       </c>
@@ -3254,7 +3296,7 @@
         <v>-2.3782000000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -3271,12 +3313,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B64" t="s">
         <v>57</v>
       </c>
@@ -3284,7 +3326,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B65" t="s">
         <v>59</v>
       </c>
@@ -3292,7 +3334,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B66" t="s">
         <v>61</v>
       </c>
@@ -3300,7 +3342,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -3311,7 +3353,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B68" t="s">
         <v>66</v>
       </c>
@@ -3327,7 +3369,7 @@
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B69" t="s">
         <v>67</v>
       </c>
@@ -3335,7 +3377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B70" t="s">
         <v>68</v>
       </c>
@@ -3343,7 +3385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B71" t="s">
         <v>69</v>
       </c>
@@ -3351,7 +3393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B72" t="s">
         <v>70</v>
       </c>
@@ -3359,7 +3401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B73" t="s">
         <v>71</v>
       </c>
@@ -3367,7 +3409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>122</v>
       </c>
@@ -3378,7 +3420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B75" t="s">
         <v>123</v>
       </c>
@@ -3386,7 +3428,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B76" t="s">
         <v>104</v>
       </c>
@@ -3394,12 +3436,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B79" t="s">
         <v>73</v>
       </c>
@@ -3407,7 +3449,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B80" t="s">
         <v>75</v>
       </c>
@@ -3415,7 +3457,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>86</v>
       </c>
@@ -3426,7 +3468,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>20</v>
       </c>
@@ -3437,7 +3479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>20</v>
       </c>
@@ -3448,7 +3490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>14</v>
       </c>
@@ -3459,7 +3501,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>14</v>
       </c>
@@ -3470,7 +3512,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>90</v>
       </c>
@@ -3484,7 +3526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>90</v>
       </c>
@@ -3495,7 +3537,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>89</v>
       </c>
@@ -3506,7 +3548,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -3520,7 +3562,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>88</v>
       </c>
@@ -3534,12 +3576,12 @@
         <v>600</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A92" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B93" t="s">
         <v>92</v>
       </c>
@@ -3547,7 +3589,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B94" t="s">
         <v>93</v>
       </c>

</xml_diff>

<commit_message>
New UnifiedLaw for 3rd run
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim_Draft_1/Code_of_Laws/UnifiedLawIteration_1.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim_Draft_1/Code_of_Laws/UnifiedLawIteration_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\REU22\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim_Draft_1\Code_of_Laws\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlg\Dropbox (ASU)\PC\Documents\GitHub\REU_MatlabSim\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim_Draft_1\Code_of_Laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF90A48-EBB0-4338-AEB3-8D934B83BAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7E26F8-30C9-43E5-972D-5E9DAE92C597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Iteration" sheetId="1" r:id="rId1"/>
@@ -786,7 +786,7 @@
   <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28:E31"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1057,10 +1057,16 @@
         <v>109</v>
       </c>
       <c r="C29">
-        <v>-2</v>
+        <v>-1.5</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="E29">
+        <v>-0.5</v>
+      </c>
+      <c r="F29">
+        <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
UnifiedLaws for Megarun 4
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim_Draft_1/Code_of_Laws/UnifiedLawIteration_1.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim_Draft_1/Code_of_Laws/UnifiedLawIteration_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlg\Dropbox (ASU)\PC\Documents\GitHub\REU_MatlabSim\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim_Draft_1\Code_of_Laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7E26F8-30C9-43E5-972D-5E9DAE92C597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0212CA11-60ED-458E-ABFD-47F40B9FB1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1464" yWindow="0" windowWidth="14292" windowHeight="11940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Iteration" sheetId="1" r:id="rId1"/>
@@ -785,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C21" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1040,13 +1040,7 @@
         <v>105</v>
       </c>
       <c r="C28">
-        <v>0.5</v>
-      </c>
-      <c r="D28">
         <v>1</v>
-      </c>
-      <c r="E28">
-        <v>1.5</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -1056,17 +1050,29 @@
       <c r="B29" t="s">
         <v>109</v>
       </c>
-      <c r="C29">
-        <v>-1.5</v>
-      </c>
-      <c r="D29">
-        <v>-1</v>
-      </c>
-      <c r="E29">
-        <v>-0.5</v>
-      </c>
-      <c r="F29">
+      <c r="C29" s="3">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="E29" s="3">
         <v>0.5</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="G29" s="3">
+        <v>1</v>
+      </c>
+      <c r="H29" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="I29" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="J29" s="3">
+        <v>1.75</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -1077,7 +1083,7 @@
         <v>111</v>
       </c>
       <c r="C30">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -1085,13 +1091,7 @@
         <v>112</v>
       </c>
       <c r="C31">
-        <v>0.5</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -1099,6 +1099,9 @@
         <v>113</v>
       </c>
       <c r="C32">
+        <v>0.5</v>
+      </c>
+      <c r="D32">
         <v>1</v>
       </c>
     </row>
@@ -1172,12 +1175,8 @@
       <c r="F38" s="2">
         <v>0.01</v>
       </c>
-      <c r="G38" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="H38" s="2">
-        <v>1</v>
-      </c>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -1261,7 +1260,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>99</v>
       </c>
@@ -1272,12 +1271,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>14</v>
       </c>
@@ -1288,7 +1287,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>45</v>
       </c>
@@ -1296,10 +1295,19 @@
         <v>44</v>
       </c>
       <c r="C53">
+        <v>5</v>
+      </c>
+      <c r="D53">
         <v>10</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E53">
+        <v>15</v>
+      </c>
+      <c r="F53">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>20</v>
       </c>
@@ -1310,7 +1318,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -1321,7 +1329,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>49</v>
       </c>
@@ -1332,7 +1340,7 @@
         <v>-0.26179938779914941</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>49</v>
       </c>
@@ -1343,7 +1351,7 @@
         <v>0.26179938779914941</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>52</v>
       </c>
@@ -1354,7 +1362,7 @@
         <v>5.7595865315812871</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>53</v>
       </c>
@@ -1362,7 +1370,7 @@
         <v>-1.8429999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>54</v>
       </c>
@@ -1370,7 +1378,7 @@
         <v>0.37819999999999998</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>55</v>
       </c>
@@ -1378,7 +1386,7 @@
         <v>-2.3782000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -1389,7 +1397,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
UnifiedLaws for Megarun 5
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim_Draft_1/Code_of_Laws/UnifiedLawIteration_1.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim_Draft_1/Code_of_Laws/UnifiedLawIteration_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlg\Dropbox (ASU)\PC\Documents\GitHub\REU_MatlabSim\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim_Draft_1\Code_of_Laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0212CA11-60ED-458E-ABFD-47F40B9FB1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16C4787-F3B7-41E9-A4FA-896DFFCE6DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="0" windowWidth="14292" windowHeight="11940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9132" yWindow="0" windowWidth="14292" windowHeight="11940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Iteration" sheetId="1" r:id="rId1"/>
@@ -785,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C21" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1020,15 +1020,18 @@
         <v>34</v>
       </c>
       <c r="C27" s="2">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="D27" s="2">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="E27" s="2">
         <v>10000</v>
       </c>
       <c r="F27" s="2">
+        <v>30000</v>
+      </c>
+      <c r="G27" s="2">
         <v>100000</v>
       </c>
       <c r="I27" s="2"/>
@@ -1051,29 +1054,15 @@
         <v>109</v>
       </c>
       <c r="C29" s="3">
-        <v>0</v>
-      </c>
-      <c r="D29" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="E29" s="3">
         <v>0.5</v>
       </c>
-      <c r="F29" s="3">
-        <v>0.75</v>
-      </c>
-      <c r="G29" s="3">
-        <v>1</v>
-      </c>
-      <c r="H29" s="3">
-        <v>1.25</v>
-      </c>
-      <c r="I29" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="J29" s="3">
-        <v>1.75</v>
-      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -1099,10 +1088,10 @@
         <v>113</v>
       </c>
       <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
         <v>0.5</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -1118,13 +1107,16 @@
         <v>0.01</v>
       </c>
       <c r="D34" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="E34" s="2">
         <v>0.1</v>
       </c>
-      <c r="E34" s="2">
+      <c r="F34" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G34" s="2">
         <v>1</v>
-      </c>
-      <c r="F34" s="2">
-        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -1135,7 +1127,16 @@
         <v>100</v>
       </c>
       <c r="C35">
+        <v>50</v>
+      </c>
+      <c r="D35">
+        <v>100</v>
+      </c>
+      <c r="E35">
         <v>200</v>
+      </c>
+      <c r="F35">
+        <v>400</v>
       </c>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
@@ -1172,9 +1173,7 @@
       <c r="E38" s="2">
         <v>1E-3</v>
       </c>
-      <c r="F38" s="2">
-        <v>0.01</v>
-      </c>
+      <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
@@ -1186,7 +1185,10 @@
         <v>118</v>
       </c>
       <c r="C39">
-        <v>200</v>
+        <v>50</v>
+      </c>
+      <c r="D39">
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -1260,7 +1262,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>99</v>
       </c>
@@ -1271,12 +1273,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>14</v>
       </c>
@@ -1287,7 +1289,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>45</v>
       </c>
@@ -1295,19 +1297,10 @@
         <v>44</v>
       </c>
       <c r="C53">
-        <v>5</v>
-      </c>
-      <c r="D53">
         <v>10</v>
       </c>
-      <c r="E53">
-        <v>15</v>
-      </c>
-      <c r="F53">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>20</v>
       </c>
@@ -1318,7 +1311,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -1329,7 +1322,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>49</v>
       </c>
@@ -1340,7 +1333,7 @@
         <v>-0.26179938779914941</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>49</v>
       </c>
@@ -1351,7 +1344,7 @@
         <v>0.26179938779914941</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>52</v>
       </c>
@@ -1362,7 +1355,7 @@
         <v>5.7595865315812871</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>53</v>
       </c>
@@ -1370,7 +1363,7 @@
         <v>-1.8429999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>54</v>
       </c>
@@ -1378,7 +1371,7 @@
         <v>0.37819999999999998</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>55</v>
       </c>
@@ -1386,7 +1379,7 @@
         <v>-2.3782000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -1397,7 +1390,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
UnifiedLaws for Megarun 6
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim_Draft_1/Code_of_Laws/UnifiedLawIteration_1.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim_Draft_1/Code_of_Laws/UnifiedLawIteration_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlg\Dropbox (ASU)\PC\Documents\GitHub\REU_MatlabSim\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim_Draft_1\Code_of_Laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16C4787-F3B7-41E9-A4FA-896DFFCE6DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73862CEF-DFCB-4A8C-9126-83D71315392C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9132" yWindow="0" windowWidth="14292" windowHeight="11940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Iteration" sheetId="1" r:id="rId1"/>
@@ -785,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -863,6 +863,9 @@
         <v>9</v>
       </c>
       <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
         <v>12</v>
       </c>
     </row>
@@ -1127,16 +1130,7 @@
         <v>100</v>
       </c>
       <c r="C35">
-        <v>50</v>
-      </c>
-      <c r="D35">
-        <v>100</v>
-      </c>
-      <c r="E35">
         <v>200</v>
-      </c>
-      <c r="F35">
-        <v>400</v>
       </c>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
@@ -1164,11 +1158,11 @@
       <c r="B38" t="s">
         <v>32</v>
       </c>
-      <c r="C38">
-        <v>0</v>
+      <c r="C38" s="2">
+        <v>-1E-3</v>
       </c>
       <c r="D38" s="2">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="E38" s="2">
         <v>1E-3</v>
@@ -1185,10 +1179,7 @@
         <v>118</v>
       </c>
       <c r="C39">
-        <v>50</v>
-      </c>
-      <c r="D39">
-        <v>100</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -1219,6 +1210,12 @@
       </c>
       <c r="C42">
         <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="D42" s="2">
+        <v>1E-22</v>
+      </c>
+      <c r="E42" s="2">
+        <v>9.9999999999999996E-24</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>